<commit_message>
control file data changed
</commit_message>
<xml_diff>
--- a/Control/Control_File.xlsx
+++ b/Control/Control_File.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Roche\Chili_Data_Acquisition\Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F068965-4BE3-4678-92C7-7485D7D2B242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80512DA4-DDAC-43D6-9A49-04683BF78F7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Downloadable_Link</t>
   </si>
@@ -46,6 +46,27 @@
   </si>
   <si>
     <t>2024-1</t>
+  </si>
+  <si>
+    <t>2024-2</t>
+  </si>
+  <si>
+    <t>2024-3</t>
+  </si>
+  <si>
+    <t>2024-4</t>
+  </si>
+  <si>
+    <t>2024-5</t>
+  </si>
+  <si>
+    <t>2024-6</t>
+  </si>
+  <si>
+    <t>2024-7</t>
+  </si>
+  <si>
+    <t>2024-8</t>
   </si>
 </sst>
 </file>
@@ -359,7 +380,7 @@
   <dimension ref="A1:A1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -375,25 +396,39 @@
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
+      <c r="A4" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
+      <c r="A5" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
+      <c r="A6" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
+      <c r="A7" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
+      <c r="A8" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
+      <c r="A9" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>

</xml_diff>

<commit_message>
filter added in part 3
</commit_message>
<xml_diff>
--- a/Control/Control_File.xlsx
+++ b/Control/Control_File.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Roche\Chili_Data_Acquisition\Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80512DA4-DDAC-43D6-9A49-04683BF78F7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D97BF20B-BF4B-416C-986F-952435E6B24B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Downloadable_Link</t>
   </si>
@@ -43,18 +43,6 @@
   </si>
   <si>
     <t>Month</t>
-  </si>
-  <si>
-    <t>2024-1</t>
-  </si>
-  <si>
-    <t>2024-2</t>
-  </si>
-  <si>
-    <t>2024-3</t>
-  </si>
-  <si>
-    <t>2024-4</t>
   </si>
   <si>
     <t>2024-5</t>
@@ -410,26 +398,6 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
     </row>

</xml_diff>

<commit_message>
control file changes 2023-1 to 2023-12
</commit_message>
<xml_diff>
--- a/Control/Control_File.xlsx
+++ b/Control/Control_File.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Roche\Chili_Data_Acquisition\Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D97BF20B-BF4B-416C-986F-952435E6B24B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7837D22B-ECA3-45ED-B0A9-69F7EC6C7139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Downloadable_Link</t>
   </si>
@@ -45,16 +45,40 @@
     <t>Month</t>
   </si>
   <si>
-    <t>2024-5</t>
+    <t>2023-1</t>
   </si>
   <si>
-    <t>2024-6</t>
+    <t>2023-2</t>
   </si>
   <si>
-    <t>2024-7</t>
+    <t>2023-3</t>
   </si>
   <si>
-    <t>2024-8</t>
+    <t>2023-4</t>
+  </si>
+  <si>
+    <t>2023-5</t>
+  </si>
+  <si>
+    <t>2023-6</t>
+  </si>
+  <si>
+    <t>2023-7</t>
+  </si>
+  <si>
+    <t>2023-8</t>
+  </si>
+  <si>
+    <t>2023-9</t>
+  </si>
+  <si>
+    <t>2023-10</t>
+  </si>
+  <si>
+    <t>2023-11</t>
+  </si>
+  <si>
+    <t>2023-12</t>
   </si>
 </sst>
 </file>
@@ -368,7 +392,7 @@
   <dimension ref="A1:A1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -398,17 +422,45 @@
         <v>6</v>
       </c>
     </row>
+    <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
+      <c r="A10" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
+      <c r="A11" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
+      <c r="A12" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
+      <c r="A13" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>

</xml_diff>

<commit_message>
Cleared the bug in part_2.py
</commit_message>
<xml_diff>
--- a/Control/Control_File.xlsx
+++ b/Control/Control_File.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Roche\Chili_Data_Acquisition\Control\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hriti\OneDrive\Desktop\Roche_Projects\Chile_Data_Acquisition\Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{134EE9A1-CF69-4D0D-8DCF-C3F1FD6738F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D06DF84B-8E7F-4617-837C-21CDE892B946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Link" sheetId="1" r:id="rId1"/>
@@ -368,7 +368,7 @@
   <dimension ref="A1:A1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
final out to mail code
</commit_message>
<xml_diff>
--- a/Control/Control_File.xlsx
+++ b/Control/Control_File.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Roche\Chili_Data_Acquisition\Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A14AF521-6B4C-4901-AB6E-4AB94C90A836}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9865C422-669F-4E78-BE0F-68B4D574D29E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -365,7 +365,7 @@
   <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
excell file drive link update
</commit_message>
<xml_diff>
--- a/Control/Control_File.xlsx
+++ b/Control/Control_File.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Roche\Chili_Data_Acquisition\Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9865C422-669F-4E78-BE0F-68B4D574D29E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C927C89-6FC7-466E-9DC0-25E5D68D941D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Downloadable_Link</t>
   </si>
@@ -53,12 +53,15 @@
   <si>
     <t>https://docs.google.com/spreadsheets/d/1nWFVPD2gPv1dxlPNOicoz_ZAO59TAT5g/edit?usp=drive_link&amp;ouid=100546778793218665121&amp;rtpof=true&amp;sd=true</t>
   </si>
+  <si>
+    <t>* (https://drive.google.com/drive/folders/1n6RlnUCTwVSI6NBtp83K1VNYRpw1P4-f)  =&gt; Locate the specified month and year link in the column Cenabast_File_Url for Cenabast from the drive link.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -82,6 +85,14 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -103,11 +114,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -362,26 +374,29 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B1000"/>
+  <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.109375" customWidth="1"/>
+    <col min="2" max="2" width="130.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -389,46 +404,46 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
     </row>
-    <row r="4" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
     </row>
-    <row r="5" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
     </row>
-    <row r="10" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
     </row>
-    <row r="11" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
     </row>
-    <row r="12" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
     </row>
-    <row r="13" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
     </row>
-    <row r="14" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
     </row>
-    <row r="15" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
     </row>
-    <row r="16" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
     </row>
     <row r="17" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
@@ -3386,5 +3401,6 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Mapping Files path change
</commit_message>
<xml_diff>
--- a/Control/Control_File.xlsx
+++ b/Control/Control_File.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Roche\Chili_Data_Acquisition\Control\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Chile_Data_Acquisition_Mercado_Publico\Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C927C89-6FC7-466E-9DC0-25E5D68D941D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F4AB2A-E5D6-40E3-86B4-5B5865DE4F2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,16 +45,16 @@
     <t>Month</t>
   </si>
   <si>
-    <t>2024-1</t>
-  </si>
-  <si>
     <t>Cenabast_File_Url</t>
   </si>
   <si>
-    <t>https://docs.google.com/spreadsheets/d/1nWFVPD2gPv1dxlPNOicoz_ZAO59TAT5g/edit?usp=drive_link&amp;ouid=100546778793218665121&amp;rtpof=true&amp;sd=true</t>
+    <t>* (https://drive.google.com/drive/folders/1n6RlnUCTwVSI6NBtp83K1VNYRpw1P4-f)  =&gt; Locate the specified month and year link in the column Cenabast_File_Url for Cenabast from the drive link.</t>
   </si>
   <si>
-    <t>* (https://drive.google.com/drive/folders/1n6RlnUCTwVSI6NBtp83K1VNYRpw1P4-f)  =&gt; Locate the specified month and year link in the column Cenabast_File_Url for Cenabast from the drive link.</t>
+    <t>https://docs.google.com/spreadsheets/d/1nk1legkPi2L_4ESXmpbCou5jaYijJcvt/edit?usp=drive_link&amp;ouid=113820234757895464527&amp;rtpof=true&amp;sd=true</t>
+  </si>
+  <si>
+    <t>2024-10</t>
   </si>
 </sst>
 </file>
@@ -376,8 +376,8 @@
   </sheetPr>
   <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -390,15 +390,15 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
datetime format changed check added
</commit_message>
<xml_diff>
--- a/Control/Control_File.xlsx
+++ b/Control/Control_File.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Chile_Data_Acquisition_Mercado_Publico\Control\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Roche\Chile_Data_Acquisition\Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F4AB2A-E5D6-40E3-86B4-5B5865DE4F2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05818C33-54AA-4FFC-80BE-60F2C5EFE1F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
     <t>https://docs.google.com/spreadsheets/d/1nk1legkPi2L_4ESXmpbCou5jaYijJcvt/edit?usp=drive_link&amp;ouid=113820234757895464527&amp;rtpof=true&amp;sd=true</t>
   </si>
   <si>
-    <t>2024-10</t>
+    <t>2024-1</t>
   </si>
 </sst>
 </file>
@@ -377,7 +377,7 @@
   <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>